<commit_message>
liability and asset import
</commit_message>
<xml_diff>
--- a/public/downloads/liability-import-template.xlsx
+++ b/public/downloads/liability-import-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jevohngentry/Desktop/invictus/public/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAF3EBDE-B34F-C845-9D75-22F23E72F93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878969C0-3A68-F849-B4BC-E23B652A74E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6860" yWindow="3540" windowWidth="27640" windowHeight="16940" xr2:uid="{BAD56F22-FF8B-294C-89A7-6D7F690EC2C2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Client ID*</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Estimated Payoff Date</t>
+  </si>
+  <si>
+    <t>Liability Owner Name</t>
   </si>
 </sst>
 </file>
@@ -447,26 +450,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0773A9-000A-C142-9AC0-9D9174053A82}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.1640625" style="1" customWidth="1"/>
-    <col min="9" max="20" width="20.83203125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="20.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.1640625" style="1" customWidth="1"/>
+    <col min="10" max="21" width="20.83203125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,24 +477,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>